<commit_message>
feat (main): skip already extracted data
</commit_message>
<xml_diff>
--- a/sample.data.xlsx
+++ b/sample.data.xlsx
@@ -13,14 +13,14 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
   <si>
     <t xml:space="preserve">Origen</t>
   </si>
@@ -31,6 +31,9 @@
     <t xml:space="preserve">Vehículo</t>
   </si>
   <si>
+    <t xml:space="preserve">Total</t>
+  </si>
+  <si>
     <t xml:space="preserve">Estado</t>
   </si>
   <si>
@@ -56,9 +59,6 @@
   </si>
   <si>
     <t xml:space="preserve">Pick Ups</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Automovil</t>
   </si>
   <si>
     <t xml:space="preserve">Camión 5 ejes</t>
@@ -143,7 +143,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -156,7 +156,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -170,6 +170,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -189,13 +193,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3:G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.42"/>
@@ -206,7 +210,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="1" width="11.54"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -218,199 +222,208 @@
       <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="E2" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F2" s="3"/>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>11</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>12</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>13</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>14</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>15</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
         <v>16</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
         <v>17</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
         <v>18</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
         <v>19</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
         <v>21</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>